<commit_message>
Add rating column to shopee_products.xlsx
</commit_message>
<xml_diff>
--- a/Crawling/data/shopee_products.xlsx
+++ b/Crawling/data/shopee_products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liewz\Documents\GitHub\CZ4034_IR\Crawling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CFBBF0-E98B-487F-AAD1-0EC060EB5181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDA7975-0C9D-4B75-BDF6-F895D18F9FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="326">
   <si>
     <t>url</t>
   </si>
@@ -1936,6 +1936,24 @@
   </si>
   <si>
     <t>$1.45 - $3.56</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -2277,19 +2295,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="51.81640625" customWidth="1"/>
-    <col min="6" max="6" width="53.36328125" customWidth="1"/>
+    <col min="7" max="7" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2306,16 +2324,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2332,16 +2353,19 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" t="s">
         <v>288</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2358,16 +2382,19 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" t="s">
         <v>282</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2384,16 +2411,19 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
+        <v>322</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2410,16 +2440,19 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
+        <v>322</v>
+      </c>
+      <c r="G5" t="s">
         <v>289</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2436,16 +2469,19 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
+        <v>322</v>
+      </c>
+      <c r="G6" t="s">
         <v>283</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>41</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2462,16 +2498,19 @@
         <v>47</v>
       </c>
       <c r="F7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G7" t="s">
         <v>290</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2488,16 +2527,19 @@
         <v>54</v>
       </c>
       <c r="F8" t="s">
+        <v>323</v>
+      </c>
+      <c r="G8" t="s">
         <v>291</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -2514,16 +2556,19 @@
         <v>61</v>
       </c>
       <c r="F9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G9" t="s">
         <v>292</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -2540,16 +2585,19 @@
         <v>67</v>
       </c>
       <c r="F10" t="s">
+        <v>322</v>
+      </c>
+      <c r="G10" t="s">
         <v>285</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>68</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2566,16 +2614,19 @@
         <v>74</v>
       </c>
       <c r="F11" t="s">
+        <v>322</v>
+      </c>
+      <c r="G11" t="s">
         <v>75</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>76</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -2592,16 +2643,19 @@
         <v>82</v>
       </c>
       <c r="F12" t="s">
+        <v>323</v>
+      </c>
+      <c r="G12" t="s">
         <v>293</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>83</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -2618,16 +2672,19 @@
         <v>89</v>
       </c>
       <c r="F13" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" t="s">
         <v>90</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>91</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -2644,16 +2701,19 @@
         <v>97</v>
       </c>
       <c r="F14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G14" t="s">
         <v>284</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>98</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -2670,16 +2730,19 @@
         <v>104</v>
       </c>
       <c r="F15" t="s">
+        <v>323</v>
+      </c>
+      <c r="G15" t="s">
         <v>105</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>12</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2696,16 +2759,19 @@
         <v>111</v>
       </c>
       <c r="F16" t="s">
+        <v>323</v>
+      </c>
+      <c r="G16" t="s">
         <v>294</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>112</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2722,16 +2788,19 @@
         <v>118</v>
       </c>
       <c r="F17" t="s">
+        <v>323</v>
+      </c>
+      <c r="G17" t="s">
         <v>295</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>119</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -2748,16 +2817,19 @@
         <v>125</v>
       </c>
       <c r="F18" t="s">
+        <v>321</v>
+      </c>
+      <c r="G18" t="s">
         <v>278</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>126</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2774,16 +2846,19 @@
         <v>132</v>
       </c>
       <c r="F19" t="s">
+        <v>322</v>
+      </c>
+      <c r="G19" t="s">
         <v>296</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>12</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -2797,16 +2872,19 @@
         <v>137</v>
       </c>
       <c r="F20" t="s">
+        <v>323</v>
+      </c>
+      <c r="G20" t="s">
         <v>297</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>138</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -2823,16 +2901,19 @@
         <v>144</v>
       </c>
       <c r="F21" t="s">
+        <v>323</v>
+      </c>
+      <c r="G21" t="s">
         <v>298</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>145</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>147</v>
       </c>
@@ -2849,16 +2930,19 @@
         <v>151</v>
       </c>
       <c r="F22" t="s">
+        <v>322</v>
+      </c>
+      <c r="G22" t="s">
         <v>299</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>152</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -2875,16 +2959,19 @@
         <v>158</v>
       </c>
       <c r="F23" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" t="s">
         <v>300</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>159</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>161</v>
       </c>
@@ -2901,16 +2988,19 @@
         <v>165</v>
       </c>
       <c r="F24" t="s">
+        <v>322</v>
+      </c>
+      <c r="G24" t="s">
         <v>286</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>166</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>168</v>
       </c>
@@ -2927,16 +3017,19 @@
         <v>172</v>
       </c>
       <c r="F25" t="s">
+        <v>322</v>
+      </c>
+      <c r="G25" t="s">
         <v>173</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>174</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -2950,16 +3043,19 @@
         <v>179</v>
       </c>
       <c r="F26" t="s">
+        <v>323</v>
+      </c>
+      <c r="G26" t="s">
         <v>301</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>180</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>182</v>
       </c>
@@ -2976,16 +3072,19 @@
         <v>186</v>
       </c>
       <c r="F27" t="s">
+        <v>322</v>
+      </c>
+      <c r="G27" t="s">
         <v>302</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>187</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>189</v>
       </c>
@@ -3002,16 +3101,19 @@
         <v>193</v>
       </c>
       <c r="F28" t="s">
+        <v>323</v>
+      </c>
+      <c r="G28" t="s">
         <v>303</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>194</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -3028,16 +3130,19 @@
         <v>200</v>
       </c>
       <c r="F29" t="s">
+        <v>323</v>
+      </c>
+      <c r="G29" t="s">
         <v>287</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>201</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>203</v>
       </c>
@@ -3054,16 +3159,19 @@
         <v>207</v>
       </c>
       <c r="F30" t="s">
+        <v>323</v>
+      </c>
+      <c r="G30" t="s">
         <v>304</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>208</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>210</v>
       </c>
@@ -3080,16 +3188,19 @@
         <v>214</v>
       </c>
       <c r="F31" t="s">
+        <v>323</v>
+      </c>
+      <c r="G31" t="s">
         <v>279</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>215</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>217</v>
       </c>
@@ -3106,16 +3217,19 @@
         <v>221</v>
       </c>
       <c r="F32" t="s">
+        <v>323</v>
+      </c>
+      <c r="G32" t="s">
         <v>305</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>222</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>224</v>
       </c>
@@ -3132,16 +3246,19 @@
         <v>228</v>
       </c>
       <c r="F33" t="s">
+        <v>322</v>
+      </c>
+      <c r="G33" t="s">
         <v>306</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>229</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>231</v>
       </c>
@@ -3158,16 +3275,19 @@
         <v>235</v>
       </c>
       <c r="F34" t="s">
+        <v>323</v>
+      </c>
+      <c r="G34" t="s">
         <v>280</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>236</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>238</v>
       </c>
@@ -3184,16 +3304,19 @@
         <v>242</v>
       </c>
       <c r="F35" t="s">
+        <v>324</v>
+      </c>
+      <c r="G35" t="s">
         <v>243</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>244</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>246</v>
       </c>
@@ -3207,16 +3330,19 @@
         <v>313</v>
       </c>
       <c r="F36" t="s">
+        <v>323</v>
+      </c>
+      <c r="G36" t="s">
         <v>307</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>247</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>249</v>
       </c>
@@ -3230,16 +3356,19 @@
         <v>252</v>
       </c>
       <c r="F37" t="s">
+        <v>325</v>
+      </c>
+      <c r="G37" t="s">
         <v>308</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>253</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -3256,16 +3385,19 @@
         <v>259</v>
       </c>
       <c r="F38" t="s">
+        <v>323</v>
+      </c>
+      <c r="G38" t="s">
         <v>309</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>260</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>262</v>
       </c>
@@ -3279,16 +3411,19 @@
         <v>265</v>
       </c>
       <c r="F39" t="s">
+        <v>323</v>
+      </c>
+      <c r="G39" t="s">
         <v>281</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>266</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>268</v>
       </c>
@@ -3305,16 +3440,19 @@
         <v>317</v>
       </c>
       <c r="F40" t="s">
+        <v>322</v>
+      </c>
+      <c r="G40" t="s">
         <v>310</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>269</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>271</v>
       </c>
@@ -3331,12 +3469,15 @@
         <v>275</v>
       </c>
       <c r="F41" t="s">
+        <v>322</v>
+      </c>
+      <c r="G41" t="s">
         <v>311</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>276</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>277</v>
       </c>
     </row>

</xml_diff>